<commit_message>
Auto stash before merge of "feature/Carmen" and "origin/feature/edward"
</commit_message>
<xml_diff>
--- a/Records28.xlsx
+++ b/Records28.xlsx
@@ -53,31 +53,31 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>4/16/2020</t>
-  </si>
-  <si>
-    <t>Atlanta</t>
+    <t>4/8/2020</t>
   </si>
   <si>
     <t>Dallas</t>
   </si>
   <si>
+    <t>NewJersey</t>
+  </si>
+  <si>
+    <t>6:00 pm</t>
+  </si>
+  <si>
     <t>4:00 pm</t>
   </si>
   <si>
-    <t>2:00 pm</t>
-  </si>
-  <si>
-    <t>Carmen</t>
-  </si>
-  <si>
-    <t>Johnson</t>
-  </si>
-  <si>
-    <t>CJ@gmail.com</t>
-  </si>
-  <si>
-    <t>123654789</t>
+    <t>Angela</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>A@aol.com</t>
+  </si>
+  <si>
+    <t>2581236548</t>
   </si>
   <si>
     <t>female</t>
@@ -174,7 +174,7 @@
     </row>
     <row r="3">
       <c r="B3" t="n">
-        <v>5.0</v>
+        <v>9.0</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -207,7 +207,7 @@
         <v>21</v>
       </c>
       <c r="M3" t="n">
-        <v>26.0</v>
+        <v>33.0</v>
       </c>
       <c r="N3" t="s">
         <v>22</v>

</xml_diff>